<commit_message>
add mission number to current mission
</commit_message>
<xml_diff>
--- a/GliderMission.xlsx
+++ b/GliderMission.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ent.dfo-mpo.ca\atlshares\MARFIS\Shares\OSD_Common\Gliders\MISSIONS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laytonc\Documents\GitHub\pilotingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83981D9D-40AF-48CB-A770-093E29063AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54473AF5-71BC-4018-9F13-8341FC9548B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25350" yWindow="1860" windowWidth="23700" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2641,80 +2641,80 @@
   <dimension ref="A1:BO74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="BA51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="BG51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BH64" sqref="BH64"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08984375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="4" customWidth="1"/>
     <col min="5" max="6" width="14" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.81640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="7.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="10.08984375" style="7" customWidth="1"/>
-    <col min="17" max="17" width="78.90625" customWidth="1"/>
-    <col min="18" max="18" width="8.08984375" customWidth="1"/>
-    <col min="19" max="19" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.77734375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="7.21875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" style="7" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="78.88671875" customWidth="1"/>
+    <col min="18" max="18" width="8.109375" customWidth="1"/>
+    <col min="19" max="19" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.81640625" customWidth="1"/>
-    <col min="22" max="22" width="11.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" customWidth="1"/>
+    <col min="22" max="22" width="11.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.54296875" style="86" customWidth="1"/>
-    <col min="28" max="28" width="20.54296875" style="86" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.54296875" style="86" customWidth="1"/>
-    <col min="30" max="30" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5546875" style="86" customWidth="1"/>
+    <col min="28" max="28" width="20.5546875" style="86" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.5546875" style="86" customWidth="1"/>
+    <col min="30" max="30" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.6328125" style="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.90625" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.6328125" style="7" customWidth="1"/>
-    <col min="37" max="37" width="7.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.36328125" style="87" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.90625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.81640625" style="87" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.81640625" style="87" customWidth="1"/>
-    <col min="45" max="45" width="12.81640625" style="87" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.81640625" style="87" customWidth="1"/>
-    <col min="47" max="47" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="17.90625" style="6" customWidth="1"/>
-    <col min="50" max="51" width="12.81640625" style="87" customWidth="1"/>
-    <col min="52" max="52" width="11.81640625" style="87" customWidth="1"/>
-    <col min="53" max="53" width="14.81640625" style="87" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15.1796875" style="87" bestFit="1" customWidth="1"/>
-    <col min="55" max="57" width="15.1796875" style="87" customWidth="1"/>
-    <col min="58" max="58" width="11.81640625" style="5" customWidth="1"/>
-    <col min="59" max="59" width="11.81640625" style="1" customWidth="1"/>
-    <col min="60" max="60" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="12.81640625" style="6" customWidth="1"/>
+    <col min="32" max="32" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.6640625" style="7" customWidth="1"/>
+    <col min="37" max="37" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.33203125" style="87" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.77734375" style="87" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.77734375" style="87" customWidth="1"/>
+    <col min="45" max="45" width="12.77734375" style="87" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.77734375" style="87" customWidth="1"/>
+    <col min="47" max="47" width="11.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.88671875" style="6" customWidth="1"/>
+    <col min="50" max="51" width="12.77734375" style="87" customWidth="1"/>
+    <col min="52" max="52" width="11.77734375" style="87" customWidth="1"/>
+    <col min="53" max="53" width="14.77734375" style="87" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.21875" style="87" bestFit="1" customWidth="1"/>
+    <col min="55" max="57" width="15.21875" style="87" customWidth="1"/>
+    <col min="58" max="58" width="11.77734375" style="5" customWidth="1"/>
+    <col min="59" max="59" width="11.77734375" style="1" customWidth="1"/>
+    <col min="60" max="60" width="12.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="12.77734375" style="6" customWidth="1"/>
     <col min="62" max="62" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="18.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="28.90625" style="4" customWidth="1"/>
-    <col min="66" max="66" width="24.90625" style="7" customWidth="1"/>
-    <col min="67" max="67" width="116.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="7.90625" customWidth="1"/>
+    <col min="63" max="63" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="18.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="28.88671875" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.88671875" style="7" customWidth="1"/>
+    <col min="67" max="67" width="116.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="7.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="107" t="s">
@@ -2774,7 +2774,7 @@
       <c r="BN1" s="25"/>
       <c r="BO1" s="30"/>
     </row>
-    <row r="2" spans="1:67" s="72" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:67" s="72" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="73" t="s">
         <v>0</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="91">
         <v>2</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>1</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>2</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>3</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>4</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>5</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>6</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>7</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>8</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>9</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>10</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>11</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23">
         <v>12</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="93">
         <v>13</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>1</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>2</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="53" t="s">
         <v>135</v>
       </c>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="BO20" s="21"/>
     </row>
-    <row r="21" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="89">
         <v>3</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="89">
         <v>3</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>4</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>5</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>6</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>7</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>8</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>9</v>
       </c>
@@ -7322,7 +7322,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="29" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>10</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>11</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>12</v>
       </c>
@@ -7823,7 +7823,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>13</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:67" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="91">
         <v>14</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="47" t="s">
         <v>284</v>
       </c>
@@ -8242,7 +8242,7 @@
       <c r="BN34" s="37"/>
       <c r="BO34" s="43"/>
     </row>
-    <row r="35" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="s">
         <v>285</v>
       </c>
@@ -8314,7 +8314,7 @@
       <c r="BN35" s="37"/>
       <c r="BO35" s="43"/>
     </row>
-    <row r="36" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <v>1</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="37" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
         <v>2</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="38" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
         <v>3</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23">
         <v>4</v>
       </c>
@@ -8994,7 +8994,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="40" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23">
         <v>5</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="23">
         <v>6</v>
       </c>
@@ -9342,7 +9342,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="42" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="23">
         <v>7</v>
       </c>
@@ -9523,7 +9523,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="43" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="23">
         <v>8</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="44" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23">
         <v>9</v>
       </c>
@@ -9863,7 +9863,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:67" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="93">
         <v>10</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="46" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>1</v>
       </c>
@@ -10207,7 +10207,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="47" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>2</v>
       </c>
@@ -10379,7 +10379,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="48" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>3</v>
       </c>
@@ -10550,7 +10550,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="49" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>4</v>
       </c>
@@ -10721,7 +10721,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="50" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <v>5</v>
       </c>
@@ -10903,7 +10903,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <v>6</v>
       </c>
@@ -11074,7 +11074,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="52" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>7</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="53" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>8</v>
       </c>
@@ -11427,7 +11427,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="54" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <v>9</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="55" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9">
         <v>10</v>
       </c>
@@ -11781,7 +11781,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="56" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>11</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="57" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>12</v>
       </c>
@@ -12140,7 +12140,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="58" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>13</v>
       </c>
@@ -12312,7 +12312,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="59" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>14</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="60" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:67" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="89">
         <v>15</v>
       </c>
@@ -12668,7 +12668,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="61" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="23">
         <v>1</v>
       </c>
@@ -12837,7 +12837,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="62" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="23">
         <v>2</v>
       </c>
@@ -13006,7 +13006,7 @@
       </c>
       <c r="BO62" s="43"/>
     </row>
-    <row r="63" spans="1:67" s="111" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:67" s="111" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="111">
         <v>3</v>
       </c>
@@ -13183,13 +13183,15 @@
       </c>
       <c r="BO63" s="120"/>
     </row>
-    <row r="64" spans="1:67" s="121" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:67" s="121" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="122"/>
       <c r="C64" s="122"/>
       <c r="D64" s="123" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="123"/>
+      <c r="E64" s="123">
+        <v>69</v>
+      </c>
       <c r="F64" s="123">
         <v>4800926</v>
       </c>
@@ -13309,7 +13311,7 @@
       <c r="BN64" s="124"/>
       <c r="BO64" s="131"/>
     </row>
-    <row r="65" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="34"/>
       <c r="C65" s="34"/>
       <c r="D65" s="35"/>
@@ -13377,7 +13379,7 @@
       <c r="BN65" s="37"/>
       <c r="BO65" s="43"/>
     </row>
-    <row r="66" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="52" t="s">
         <v>99</v>
       </c>
@@ -13441,7 +13443,7 @@
       <c r="BN66" s="48"/>
       <c r="BO66" s="30"/>
     </row>
-    <row r="67" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="34"/>
       <c r="C67" s="34"/>
       <c r="D67" s="35"/>
@@ -13511,7 +13513,7 @@
       <c r="BN67" s="48"/>
       <c r="BO67" s="30"/>
     </row>
-    <row r="68" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B68" s="34"/>
       <c r="C68" s="34"/>
       <c r="D68" s="35"/>
@@ -13589,7 +13591,7 @@
       <c r="BN68" s="48"/>
       <c r="BO68" s="30"/>
     </row>
-    <row r="69" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B69" s="34"/>
       <c r="C69" s="34"/>
       <c r="D69" s="35"/>
@@ -13667,7 +13669,7 @@
       <c r="BN69" s="48"/>
       <c r="BO69" s="30"/>
     </row>
-    <row r="70" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="34"/>
       <c r="C70" s="34"/>
       <c r="D70" s="35"/>
@@ -13747,7 +13749,7 @@
       <c r="BN70" s="48"/>
       <c r="BO70" s="30"/>
     </row>
-    <row r="71" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:67" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="34"/>
       <c r="C71" s="34"/>
       <c r="D71" s="35"/>
@@ -13825,7 +13827,7 @@
       <c r="BN71" s="48"/>
       <c r="BO71" s="30"/>
     </row>
-    <row r="72" spans="2:67" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:67" x14ac:dyDescent="0.3">
       <c r="BH72" s="102" t="s">
         <v>283</v>
       </c>
@@ -13845,7 +13847,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="73" spans="2:67" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:67" x14ac:dyDescent="0.3">
       <c r="BH73" s="46" t="s">
         <v>328</v>
       </c>
@@ -13857,7 +13859,7 @@
       <c r="BL73" s="29"/>
       <c r="BM73" s="29"/>
     </row>
-    <row r="74" spans="2:67" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:67" x14ac:dyDescent="0.3">
       <c r="BH74" s="46"/>
       <c r="BI74" s="46"/>
       <c r="BJ74" s="46"/>
@@ -13877,7 +13879,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13890,7 +13892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix calib date for recent mission
</commit_message>
<xml_diff>
--- a/GliderMission.xlsx
+++ b/GliderMission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laytonc\Documents\GitHub\pilotingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54473AF5-71BC-4018-9F13-8341FC9548B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D09B470-D75F-440C-AA78-3A6B7940FDD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2641,10 +2641,10 @@
   <dimension ref="A1:BO74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="BG51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AL51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomRight" activeCell="AQ65" sqref="AQ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13262,7 +13262,7 @@
         <v>72</v>
       </c>
       <c r="AQ64" s="126" t="s">
-        <v>526</v>
+        <v>502</v>
       </c>
       <c r="AR64" s="126"/>
       <c r="AS64" s="126"/>

</xml_diff>

<commit_message>
sea019 m120 to 121
</commit_message>
<xml_diff>
--- a/GliderMission.xlsx
+++ b/GliderMission.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="none" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ent.dfo-mpo.ca\atlshares\MARFIS\Shares\OSD_Common\Gliders\MISSIONS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laytonc\Documents\GitHub\pilotingApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C7B084-DB10-4891-9680-C5EFE0AA08B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF06A0B-F6C0-4020-9608-2631A6AB166A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8304" yWindow="228" windowWidth="15576" windowHeight="11496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2847,81 +2847,81 @@
   <dimension ref="A1:BP87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AM59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AW59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AP70" sqref="AP70:AR70"/>
+      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="3" width="15.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="2" max="3" width="15.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="14" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.81640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.77734375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="7" customWidth="1"/>
-    <col min="15" max="15" width="7.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.81640625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" style="7" customWidth="1"/>
-    <col min="18" max="18" width="78.81640625" customWidth="1"/>
-    <col min="19" max="19" width="8.1796875" customWidth="1"/>
-    <col min="20" max="20" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" style="7" customWidth="1"/>
+    <col min="18" max="18" width="78.77734375" customWidth="1"/>
+    <col min="19" max="19" width="8.21875" customWidth="1"/>
+    <col min="20" max="20" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.81640625" customWidth="1"/>
-    <col min="23" max="23" width="11.1796875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.77734375" customWidth="1"/>
+    <col min="23" max="23" width="11.21875" style="7" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.54296875" style="82" customWidth="1"/>
-    <col min="29" max="29" width="20.54296875" style="82" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.54296875" style="82" customWidth="1"/>
-    <col min="31" max="31" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5546875" style="82" customWidth="1"/>
+    <col min="29" max="29" width="20.5546875" style="82" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.5546875" style="82" customWidth="1"/>
+    <col min="31" max="31" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.54296875" style="7" customWidth="1"/>
-    <col min="38" max="38" width="7.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.453125" style="83" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.81640625" style="83" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.81640625" style="83" customWidth="1"/>
-    <col min="46" max="46" width="12.81640625" style="83" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.81640625" style="83" customWidth="1"/>
-    <col min="48" max="48" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.81640625" style="6" customWidth="1"/>
-    <col min="51" max="52" width="12.81640625" style="83" customWidth="1"/>
-    <col min="53" max="53" width="11.81640625" style="83" customWidth="1"/>
-    <col min="54" max="54" width="14.81640625" style="83" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.1796875" style="83" bestFit="1" customWidth="1"/>
-    <col min="56" max="58" width="15.1796875" style="83" customWidth="1"/>
-    <col min="59" max="59" width="11.81640625" style="5" customWidth="1"/>
-    <col min="60" max="60" width="11.81640625" style="1" customWidth="1"/>
-    <col min="61" max="61" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.81640625" style="6" customWidth="1"/>
+    <col min="33" max="33" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.5546875" style="7" customWidth="1"/>
+    <col min="38" max="38" width="7.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.44140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="16.77734375" style="83" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.77734375" style="83" customWidth="1"/>
+    <col min="46" max="46" width="12.77734375" style="83" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.77734375" style="83" customWidth="1"/>
+    <col min="48" max="48" width="11.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.77734375" style="6" customWidth="1"/>
+    <col min="51" max="52" width="12.77734375" style="83" customWidth="1"/>
+    <col min="53" max="53" width="11.77734375" style="83" customWidth="1"/>
+    <col min="54" max="54" width="14.77734375" style="83" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.21875" style="83" bestFit="1" customWidth="1"/>
+    <col min="56" max="58" width="15.21875" style="83" customWidth="1"/>
+    <col min="59" max="59" width="11.77734375" style="5" customWidth="1"/>
+    <col min="60" max="60" width="11.77734375" style="1" customWidth="1"/>
+    <col min="61" max="61" width="12.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.77734375" style="6" customWidth="1"/>
     <col min="63" max="63" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="19" style="4" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="25.7265625" style="7" customWidth="1"/>
-    <col min="68" max="68" width="116.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="7.81640625" customWidth="1"/>
+    <col min="67" max="67" width="25.77734375" style="7" customWidth="1"/>
+    <col min="68" max="68" width="116.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
       <c r="D1" s="103" t="s">
@@ -2981,7 +2981,7 @@
       <c r="BO1" s="25"/>
       <c r="BP1" s="30"/>
     </row>
-    <row r="2" spans="1:68" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:68" s="68" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="87">
         <v>2</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>1</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>2</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>3</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>4</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>5</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>6</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>7</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>8</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>9</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>10</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>11</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23">
         <v>12</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="89">
         <v>13</v>
       </c>
@@ -5767,7 +5767,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>1</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <v>2</v>
       </c>
@@ -6105,7 +6105,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="49" t="s">
         <v>134</v>
       </c>
@@ -6182,7 +6182,7 @@
       </c>
       <c r="BP20" s="21"/>
     </row>
-    <row r="21" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="85">
         <v>3</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="22" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="85">
         <v>3</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>4</v>
       </c>
@@ -6700,7 +6700,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
         <v>5</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
         <v>6</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>7</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
         <v>8</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>9</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="29" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
         <v>10</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>11</v>
       </c>
@@ -7889,7 +7889,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="31" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>12</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="32" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9">
         <v>13</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:68" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="87">
         <v>14</v>
       </c>
@@ -8411,7 +8411,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="47" t="s">
         <v>282</v>
       </c>
@@ -8484,7 +8484,7 @@
       <c r="BO34" s="37"/>
       <c r="BP34" s="43"/>
     </row>
-    <row r="35" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="s">
         <v>283</v>
       </c>
@@ -8557,7 +8557,7 @@
       <c r="BO35" s="37"/>
       <c r="BP35" s="43"/>
     </row>
-    <row r="36" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <v>1</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
         <v>2</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
         <v>3</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="39" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="23">
         <v>4</v>
       </c>
@@ -9241,7 +9241,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="40" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="23">
         <v>5</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="41" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="23">
         <v>6</v>
       </c>
@@ -9591,7 +9591,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="23">
         <v>7</v>
       </c>
@@ -9773,7 +9773,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="43" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="23">
         <v>8</v>
       </c>
@@ -9945,7 +9945,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="44" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23">
         <v>9</v>
       </c>
@@ -10115,7 +10115,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="45" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:68" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="89">
         <v>10</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="46" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
         <v>1</v>
       </c>
@@ -10461,7 +10461,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="47" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>2</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="48" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>3</v>
       </c>
@@ -10806,7 +10806,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="49" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>4</v>
       </c>
@@ -10978,7 +10978,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="50" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <v>5</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="51" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <v>6</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="52" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9">
         <v>7</v>
       </c>
@@ -11505,7 +11505,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="53" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9">
         <v>8</v>
       </c>
@@ -11688,7 +11688,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="54" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9">
         <v>9</v>
       </c>
@@ -11870,7 +11870,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="55" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9">
         <v>10</v>
       </c>
@@ -12044,7 +12044,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>11</v>
       </c>
@@ -12218,7 +12218,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9">
         <v>12</v>
       </c>
@@ -12405,7 +12405,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="58" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>13</v>
       </c>
@@ -12578,7 +12578,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9">
         <v>14</v>
       </c>
@@ -12750,7 +12750,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="60" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="85">
         <v>15</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="61" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="23">
         <v>1</v>
       </c>
@@ -13108,7 +13108,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="62" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="23">
         <v>2</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="63" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="23">
         <v>3</v>
       </c>
@@ -13460,7 +13460,7 @@
       </c>
       <c r="BP63" s="43"/>
     </row>
-    <row r="64" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="23">
         <v>4</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="65" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:68" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="68">
         <v>5</v>
       </c>
@@ -13812,7 +13812,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="66" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>1</v>
       </c>
@@ -13995,7 +13995,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="67" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="9">
         <v>2</v>
       </c>
@@ -14170,7 +14170,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="68" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="9">
         <v>3</v>
       </c>
@@ -14345,7 +14345,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="69" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="9">
         <v>4</v>
       </c>
@@ -14530,14 +14530,14 @@
         <v>593</v>
       </c>
     </row>
-    <row r="70" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="107"/>
       <c r="C70" s="20"/>
       <c r="D70" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E70" s="14">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F70" s="14">
         <v>4800925</v>
@@ -14661,7 +14661,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="71" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
       <c r="D71" s="14" t="s">
@@ -14744,7 +14744,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="72" spans="1:68" s="141" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:68" s="141" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="142"/>
       <c r="C72" s="142"/>
       <c r="D72" s="142"/>
@@ -14813,7 +14813,7 @@
       <c r="BO72" s="143"/>
       <c r="BP72" s="148"/>
     </row>
-    <row r="73" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="133"/>
       <c r="C73" s="133"/>
       <c r="D73" s="133"/>
@@ -14882,7 +14882,7 @@
       <c r="BO73" s="134"/>
       <c r="BP73" s="139"/>
     </row>
-    <row r="74" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B74" s="133"/>
       <c r="C74" s="133"/>
       <c r="D74" s="133"/>
@@ -14951,7 +14951,7 @@
       <c r="BO74" s="134"/>
       <c r="BP74" s="139"/>
     </row>
-    <row r="75" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B75" s="133"/>
       <c r="C75" s="133"/>
       <c r="D75" s="133"/>
@@ -15020,7 +15020,7 @@
       <c r="BO75" s="134"/>
       <c r="BP75" s="139"/>
     </row>
-    <row r="76" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B76" s="133"/>
       <c r="C76" s="133"/>
       <c r="D76" s="133"/>
@@ -15089,7 +15089,7 @@
       <c r="BO76" s="134"/>
       <c r="BP76" s="139"/>
     </row>
-    <row r="77" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B77" s="133"/>
       <c r="C77" s="133"/>
       <c r="D77" s="133"/>
@@ -15158,7 +15158,7 @@
       <c r="BO77" s="134"/>
       <c r="BP77" s="139"/>
     </row>
-    <row r="78" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B78" s="133"/>
       <c r="C78" s="133"/>
       <c r="D78" s="133"/>
@@ -15229,7 +15229,7 @@
       <c r="BO78" s="134"/>
       <c r="BP78" s="139"/>
     </row>
-    <row r="79" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B79" s="133"/>
       <c r="C79" s="133"/>
       <c r="D79" s="133"/>
@@ -15308,7 +15308,7 @@
       <c r="BO79" s="134"/>
       <c r="BP79" s="139"/>
     </row>
-    <row r="80" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B80" s="129"/>
       <c r="C80" s="129"/>
       <c r="D80" s="129"/>
@@ -15375,7 +15375,7 @@
       <c r="BO80" s="82"/>
       <c r="BP80" s="132"/>
     </row>
-    <row r="81" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B81" s="129"/>
       <c r="C81" s="129"/>
       <c r="D81" s="129"/>
@@ -15444,7 +15444,7 @@
       <c r="BO81" s="82"/>
       <c r="BP81" s="132"/>
     </row>
-    <row r="82" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="129"/>
       <c r="C82" s="129"/>
       <c r="D82" s="129"/>
@@ -15511,7 +15511,7 @@
       <c r="BO82" s="82"/>
       <c r="BP82" s="132"/>
     </row>
-    <row r="83" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B83" s="129"/>
       <c r="C83" s="129"/>
       <c r="D83" s="129"/>
@@ -15580,7 +15580,7 @@
       <c r="BO83" s="82"/>
       <c r="BP83" s="132"/>
     </row>
-    <row r="84" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B84" s="129"/>
       <c r="C84" s="129"/>
       <c r="D84" s="129"/>
@@ -15641,7 +15641,7 @@
       <c r="BO84" s="82"/>
       <c r="BP84" s="132"/>
     </row>
-    <row r="85" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B85" s="129"/>
       <c r="C85" s="129"/>
       <c r="D85" s="129"/>
@@ -15698,7 +15698,7 @@
       <c r="BO85" s="82"/>
       <c r="BP85" s="132"/>
     </row>
-    <row r="86" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B86" s="129"/>
       <c r="C86" s="129"/>
       <c r="D86" s="129"/>
@@ -15754,7 +15754,7 @@
       <c r="BO86" s="82"/>
       <c r="BP86" s="132"/>
     </row>
-    <row r="87" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:68" s="128" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B87" s="129"/>
       <c r="C87" s="129"/>
       <c r="D87" s="129"/>
@@ -15824,17 +15824,17 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="4" spans="1:5" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:5" s="23" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="117" t="s">
         <v>555</v>
       </c>
@@ -15851,7 +15851,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="114" t="s">
         <v>19</v>
       </c>
@@ -15868,7 +15868,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>60</v>
       </c>
@@ -15885,7 +15885,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="121" t="s">
         <v>123</v>
       </c>
@@ -15902,7 +15902,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
         <v>179</v>
       </c>
@@ -15919,7 +15919,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="121" t="s">
         <v>240</v>
       </c>
@@ -15936,7 +15936,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="121" t="s">
         <v>312</v>
       </c>
@@ -15953,7 +15953,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>422</v>
       </c>
@@ -15970,7 +15970,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="34" t="s">
         <v>500</v>
       </c>
@@ -15987,7 +15987,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="111"/>
     </row>
   </sheetData>
@@ -16002,7 +16002,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>